<commit_message>
Schulferien - unnötige Zeilen gelöscht
</commit_message>
<xml_diff>
--- a/Daten/Schulferien/FER2011_12.xlsx
+++ b/Daten/Schulferien/FER2011_12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achim\OneDrive\Hochschule\DSC_Semester4\Data Analytics and Business Intelligence 2\Projekt\dabi2-project\Daten\Schulferien\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93680e6007ede3e3/Hochschule/DSC_Semester4/Data Analytics and Business Intelligence 2/Projekt/dabi2-project/Daten/Schulferien/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA8B58E-EFC7-4E0D-954D-210AF3559279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8DA8B58E-EFC7-4E0D-954D-210AF3559279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{762CBEB0-E3A6-4CF7-93D2-BD9E03FBBBAB}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Land
 (in Klammern Zahl der
@@ -434,151 +434,12 @@
   <si>
     <t>23.07. - 31.08.</t>
   </si>
-  <si>
-    <t>Stand: 19.04.2012</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">Angegeben ist jeweils der erste und letzte Ferientag; angegeben ist auch die Anzahl der beweglichen Ferientage. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Nachträgliche Änderungen einzelner Länder sind vorbehalten.</t>
-    </r>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Während die Kultusministerkonferenz die Sommerferien langfristig vereinbart, werden die übrigen Ferientermine von den Ländern selbst bestimmt. Die Länder übermitteln ihre Ferientermine
-dem Sekretariat der Kultusministerkonferenz, das sie als Übersicht veröffentlicht.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> Die Veröffentlichung erfolgt fortlaufend. Es wird daher gebeten, von Nachfragen beim Sekretariat über ggf. noch nicht vorliegende Ferientermine abzusehen. Auf den Webseiten der</t>
-    </r>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Schulverwaltungen der einzelnen Länder finden Sie ggf. weitergehende Ferienplanungen für das jeweilige Land.</t>
-  </si>
-  <si>
-    <t>BW – Reformationsfest ist schulfrei.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>MV - Abweichende Ferientermine in den beruflichen Schulen.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>SH - Auf den Inseln Sylt, Föhr, Amrum und Helgoland sowie auf den Halligen gelten für die Sommer- und Herbstferien Sonderregelungen.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -635,19 +496,6 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -721,29 +569,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,10 +876,10 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A18" sqref="A18:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27"/>
     <col min="2" max="2" width="38"/>
@@ -1040,7 +888,7 @@
     <col min="7" max="7" width="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1086,7 +934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="41" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1109,7 +957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1132,7 +980,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1155,7 +1003,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1178,7 +1026,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1049,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1072,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -1247,7 +1095,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -1270,7 +1118,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>70</v>
       </c>
@@ -1293,7 +1141,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>77</v>
       </c>
@@ -1316,7 +1164,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
@@ -1339,7 +1187,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>91</v>
       </c>
@@ -1362,7 +1210,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>98</v>
       </c>
@@ -1385,7 +1233,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>105</v>
       </c>
@@ -1408,7 +1256,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>112</v>
       </c>
@@ -1431,177 +1279,93 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="8">
-        <v>2</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="8">
-        <v>3</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="14">
-        <v>4</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+    <row r="18" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:G22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="B28:G28"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:G22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>